<commit_message>
create user route in server
</commit_message>
<xml_diff>
--- a/server design.xlsx
+++ b/server design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Playground\socket.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{822719B2-5E82-4E25-8546-3482097B9E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14AEE79-61EA-41AE-835E-450BD922DD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4AE59850-DFE1-43A2-903C-F260D8E7E672}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Backend design</t>
   </si>
@@ -93,9 +93,6 @@
     <t>returned value - refresh and access tokens and user object with username, user id and image URL</t>
   </si>
   <si>
-    <t>/new</t>
-  </si>
-  <si>
     <t>create new chat</t>
   </si>
   <si>
@@ -103,6 +100,24 @@
   </si>
   <si>
     <t>get chats that current user are in them by query</t>
+  </si>
+  <si>
+    <t>/refreshToken</t>
+  </si>
+  <si>
+    <t>create new accessToken from refreshToken</t>
+  </si>
+  <si>
+    <t>returned value - new chat id, need authentication!</t>
+  </si>
+  <si>
+    <t>/data</t>
+  </si>
+  <si>
+    <t>get user data according accessToken</t>
+  </si>
+  <si>
+    <t>returned value - user object with username, user id and image URL</t>
   </si>
 </sst>
 </file>
@@ -383,54 +398,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -454,6 +421,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4FC568-7198-4C34-A9C8-F46C83B6C4D0}">
   <dimension ref="B1:P15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -784,138 +799,138 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="23"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="26"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="2:16" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="26"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="9" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="9" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="12"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="17"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="28" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -924,10 +939,10 @@
       <c r="H8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -936,139 +951,155 @@
       <c r="L8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="23" t="s">
+      <c r="M8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="70" x14ac:dyDescent="0.3">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="42" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="22"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
+      <c r="D10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="7"/>
+      <c r="J10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="22"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="22"/>
+      <c r="M10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="42" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="6"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="22"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="23"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="22"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="22"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="23"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="22"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="22"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="22"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="6"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="23"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="22"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="6"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="23"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="2:16" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="26"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>